<commit_message>
just put in the file names
</commit_message>
<xml_diff>
--- a/testData/hkor_test.xlsx
+++ b/testData/hkor_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lesleycheung/Desktop/mazen/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lesleycheung/Desktop/mazen/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C06C64-6A7B-4047-89DB-D837D12BEF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F735147-3DB6-9743-BAC4-6E7117FDB002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16220" yWindow="-21100" windowWidth="19200" windowHeight="21100" xr2:uid="{4C225EBC-E217-48E2-B71C-D347E4CDAFCD}"/>
   </bookViews>
@@ -631,7 +631,7 @@
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I14"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>